<commit_message>
Version 3.ea: Fixed BC0 counter, declared as 12 bits.  No TMR.
Former-commit-id: 33fedb52c5f2933566f30803429c2f9fedbdc4d7
</commit_message>
<xml_diff>
--- a/ResourceUsage.xlsx
+++ b/ResourceUsage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="12120" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Resource Usage" sheetId="1" r:id="rId1"/>
@@ -174,10 +174,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -230,17 +230,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Percentage of Register</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
               <a:t> and LUT usage</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -324,7 +325,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -346,6 +347,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -452,7 +454,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -474,6 +476,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -543,11 +546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="203574576"/>
-        <c:axId val="203188608"/>
+        <c:axId val="187278688"/>
+        <c:axId val="187283168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="203574576"/>
+        <c:axId val="187278688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,12 +578,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -590,7 +590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203188608"/>
+        <c:crossAx val="187283168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,7 +598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203188608"/>
+        <c:axId val="187283168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -647,12 +647,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -662,7 +659,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203574576"/>
+        <c:crossAx val="187278688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -677,6 +674,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -793,14 +791,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Resource Usage Increase When Adding Selective</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
               <a:t> TMR</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1000,7 +998,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -1093,11 +1091,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="203305040"/>
-        <c:axId val="203305936"/>
+        <c:axId val="187441800"/>
+        <c:axId val="187444232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="203305040"/>
+        <c:axId val="187441800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,12 +1123,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1140,7 +1135,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203305936"/>
+        <c:crossAx val="187444232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1148,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203305936"/>
+        <c:axId val="187444232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,12 +1191,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1211,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203305040"/>
+        <c:crossAx val="187441800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1348,6 +1340,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1420,7 +1413,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -1442,6 +1435,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1583,11 +1577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="203379152"/>
-        <c:axId val="203381584"/>
+        <c:axId val="187460512"/>
+        <c:axId val="187460896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="203379152"/>
+        <c:axId val="187460512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,12 +1609,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1630,7 +1621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203381584"/>
+        <c:crossAx val="187460896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1638,7 +1629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203381584"/>
+        <c:axId val="187460896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1687,12 +1678,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1702,7 +1690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203379152"/>
+        <c:crossAx val="187460512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -3609,7 +3597,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3620,7 +3608,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3631,7 +3619,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672286" cy="6295571"/>
+    <xdr:ext cx="8663548" cy="6289301"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3658,7 +3646,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663548" cy="6289301"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3685,7 +3673,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671034" cy="6289784"/>
+    <xdr:ext cx="8663548" cy="6289301"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3973,7 +3961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -3983,35 +3971,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="5"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="4"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4053,7 +4041,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -4109,7 +4097,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -4132,7 +4120,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -4155,7 +4143,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -4211,7 +4199,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -4265,7 +4253,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -4995,14 +4983,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>